<commit_message>
"nancy" recovery from branches is now completed, including corrections on data orders of magnitude; new explanatory plots and figures with mean values and errors.
</commit_message>
<xml_diff>
--- a/15N_experiment/15N_branches/applied_15N_per_length_and_by_surface.xlsx
+++ b/15N_experiment/15N_branches/applied_15N_per_length_and_by_surface.xlsx
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>15N application on branches: numbers</t>
-  </si>
-  <si>
-    <t>15N-NH4NO3</t>
   </si>
   <si>
     <t>total 15N in mg</t>
@@ -136,13 +133,16 @@
       <t>N rec (%)</t>
     </r>
   </si>
+  <si>
+    <t>15N-NH4NO3 (mg)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -272,12 +272,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,7 +562,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:J14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,28 +581,28 @@
     </row>
     <row r="2" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -617,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3" s="7">
         <v>1.4172549999999999</v>
@@ -632,13 +632,13 @@
         <v>5.4953000000000003</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J4" s="8">
         <v>4.7865120000000001</v>
       </c>
       <c r="K4" s="4">
-        <f t="shared" ref="K4:K6" si="0">J4*(54/$D$6)*1000</f>
+        <f t="shared" ref="K4:K5" si="0">J4*(54/$D$6)*1000</f>
         <v>5.3908447943351385</v>
       </c>
     </row>
@@ -647,7 +647,7 @@
         <v>5.4074999999999998</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="7">
         <v>1.9090119999999999</v>
@@ -670,11 +670,11 @@
         <v>47946.408746846093</v>
       </c>
       <c r="E6" s="1">
-        <f>C6/20.99</f>
-        <v>0.46370276205858774</v>
+        <f>C6/(20.99*100)</f>
+        <v>4.6370276205858771E-3</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" s="8">
         <v>5.210318</v>
@@ -691,106 +691,106 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="I10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="12">
+        <v>17</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="11">
         <v>117.2</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="11">
         <v>74.900000000000006</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="11">
         <v>18.100000000000001</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="11">
         <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="12">
+      <c r="G12" s="11">
         <v>20.6</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <v>24.76</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="11">
         <v>288</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="11">
         <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="12">
+        <v>17</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="11">
         <v>13.41</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="11">
         <v>7.17</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="11">
         <v>3.12</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="11">
         <v>20.77</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="12">
+        <v>18</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="11">
         <v>1.9</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="11">
         <v>1.4</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="11">
         <v>5.21</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="11">
         <v>4.78</v>
       </c>
     </row>

</xml_diff>